<commit_message>
edicao da planilha de contribuicao
</commit_message>
<xml_diff>
--- a/SI401_ContribuicaoIndividualTrabalho_2021.xlsx
+++ b/SI401_ContribuicaoIndividualTrabalho_2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fischer\Desktop\UNICAMP\4SEM\WEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fischer\Desktop\Projeto-SI401\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -122,13 +122,13 @@
     <t>Robson Henrique Fischer</t>
   </si>
   <si>
-    <t>Contribuiu com o desenvolvimento da pagina de usuarios.</t>
-  </si>
-  <si>
     <t>Contribuiu com o desenvolvimento da pagina login e jogo.</t>
   </si>
   <si>
-    <t>Contribuiu com o desenvolvimento da pagina de ranking.</t>
+    <t>Contribuiu com o desenvolvimento da pagina de ranking e histórico.</t>
+  </si>
+  <si>
+    <t>Contribuiu com o desenvolvimento da pagina de usuários.</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
         <v>0.34</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="31">
         <f>IF(D9="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D9),1),"Erro"))</f>
@@ -975,7 +975,7 @@
         <v>0.33</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="31">
         <f t="shared" ref="F10:F13" si="0">IF(D10="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D10),1),"Erro"))</f>
@@ -996,7 +996,7 @@
         <v>0.33</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F11" s="31">
         <f t="shared" si="0"/>
@@ -1060,7 +1060,7 @@
       <c r="E16" s="37"/>
       <c r="F16" s="6">
         <f ca="1">NOW()</f>
-        <v>44459.810630208332</v>
+        <v>44460.898523842596</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1535,18 +1535,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1569,14 +1569,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDB3412-F176-463C-9CD3-ADF26C83D016}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0537F2A3-82D8-4D11-AF44-B60EFF661ED7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1591,4 +1583,12 @@
     <ds:schemaRef ds:uri="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDB3412-F176-463C-9CD3-ADF26C83D016}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>